<commit_message>
add 9 new script
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.60.30.90_DailyForGlobalStatusPolling.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.60.30.90_DailyForGlobalStatusPolling.xlsx
@@ -4565,8 +4565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>